<commit_message>
dodanie opisu pod silnikiem
</commit_message>
<xml_diff>
--- a/konfigurator.xlsx
+++ b/konfigurator.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48697\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48697\Desktop\zwinne - konfigurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637FFE97-901C-4902-B81B-C8520AE37171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FAC0EE-666C-4411-99AB-3D14E3928065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46C60DD0-B569-4309-A117-32352B2F0D56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{46C60DD0-B569-4309-A117-32352B2F0D56}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz2" sheetId="2" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Arkusz1!$A$25:$F$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="67">
   <si>
     <t>czarny</t>
   </si>
@@ -142,6 +144,102 @@
   </si>
   <si>
     <t>fwd</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Kategoria</t>
+  </si>
+  <si>
+    <t>Rodzaj</t>
+  </si>
+  <si>
+    <t>Opis</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Nazwa</t>
+  </si>
+  <si>
+    <t>Wersja</t>
+  </si>
+  <si>
+    <t>Wykluczajacy</t>
+  </si>
+  <si>
+    <t>opis</t>
+  </si>
+  <si>
+    <t>Skrzynia manuala, napęd FWD, zużycie paliwa średnie: 5.2 l/100 km, średnia emisja CO2: 115.0 g/km.</t>
+  </si>
+  <si>
+    <t>Skrzynia manuala, napęd FWD, zużycie paliwa średnie: 4.6 l/100 km, średnia emisja CO2: 119.0 g/km.</t>
+  </si>
+  <si>
+    <t>Skrzynia manuala, napęd FWD, zużycie paliwa średnie: 4.3 l/100 km, średnia emisja CO2: 125.0 g/km.</t>
+  </si>
+  <si>
+    <t>Skrzynia automatyczna, napęd RWD, zużycie paliwa średnie: 4.5 l/100 km, średnia emisja CO2: 127.0 g/km.</t>
+  </si>
+  <si>
+    <t>Skrzynia automatyczna, napęd AWD, zużycie prądu 15 kWh/100 km</t>
+  </si>
+  <si>
+    <t>Czarny to synonim uniwersalności, a zarazem elegancja</t>
+  </si>
+  <si>
+    <t>Srebrny to synonim dostatku i prestiżu</t>
+  </si>
+  <si>
+    <t>Szary to rozwaga i ostrożność</t>
+  </si>
+  <si>
+    <t>Jeśli przywiązujesz wagę do walorów estetycznych ten kolor jest dla Ciebie!</t>
+  </si>
+  <si>
+    <t>Jesteś łowcą przygód? Żóły to jest to!</t>
+  </si>
+  <si>
+    <t>Lubisz wyróżniać się w tłumie? Ten kolor jest idealny dla Ciebie!</t>
+  </si>
+  <si>
+    <t>letnie 17'</t>
+  </si>
+  <si>
+    <t>Fenomenalna przyczepność, krótka droga hamowania</t>
+  </si>
+  <si>
+    <t>letnie 18'</t>
+  </si>
+  <si>
+    <t>dodatki</t>
+  </si>
+  <si>
+    <t>Przyciemnianie szyb poprawia komfort jazdy, zabezpiecza auto przed nagrzewaniem</t>
+  </si>
+  <si>
+    <t>Chromowane listwy wykonane z polerowanej stali nierdzewnej dodadzą elegancji oraz podkreślą wyjątkowy charakter Twojego auta</t>
+  </si>
+  <si>
+    <t>Relingi dachowe to element, który znacząco ułatwia montaż dodatkowego bagażnika na dachu samochodu</t>
+  </si>
+  <si>
+    <t>Dokładka wykonana jest z włókna węglowego i jest w błyszczącym wykończeniu</t>
+  </si>
+  <si>
+    <t>Zapewniają oryginalny wygląd auta, ale też polepsza jego własności aerodynamiczne</t>
+  </si>
+  <si>
+    <t>System wspomagający parkowanie samochodów, cały manewr jest wykonywany automatycznie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dożywotnia aktualizacja map, informacja o parkingach </t>
+  </si>
+  <si>
+    <t>Elektryczna regulacja fotela kierowcy, zapamiętuje do trzech ustawień</t>
   </si>
 </sst>
 </file>
@@ -534,11 +632,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B12B9415-A764-40AF-BFDB-3957A0A7263A}">
   <dimension ref="A1:AH93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1433,7 +1531,7 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
-        <f t="shared" ref="A82:A84" si="11">_xlfn.CONCAT("('",Z4,"',",AB$2,",",$Z$1,",",AB4,",",$AA$1,"),")</f>
+        <f t="shared" ref="A82:A83" si="11">_xlfn.CONCAT("('",Z4,"',",AB$2,",",$Z$1,",",AB4,",",$AA$1,"),")</f>
         <v>('ekoskóra',2,6,3500,1),</v>
       </c>
     </row>
@@ -1451,7 +1549,7 @@
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
-        <f t="shared" ref="A85:A87" si="12">_xlfn.CONCAT("('",Z4,"',",AC$2,",",$Z$1,",",AC4,",",$AA$1,"),")</f>
+        <f t="shared" ref="A85:A86" si="12">_xlfn.CONCAT("('",Z4,"',",AC$2,",",$Z$1,",",AC4,",",$AA$1,"),")</f>
         <v>('ekoskóra',3,6,4000,1),</v>
       </c>
     </row>
@@ -1487,7 +1585,7 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="str">
-        <f t="shared" ref="A91:A93" si="14">_xlfn.CONCAT("('",AE4,"',",AG$2,",",$AE$1,",",AG4,",",$AF$1,"),")</f>
+        <f t="shared" ref="A91:A92" si="14">_xlfn.CONCAT("('",AE4,"',",AG$2,",",$AE$1,",",AG4,",",$AF$1,"),")</f>
         <v>('Navigation',2,7,3000,0),</v>
       </c>
     </row>
@@ -1507,4 +1605,1782 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05637BF-DA77-47CE-B145-BF447AC71CC8}">
+  <dimension ref="A1:K83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D47" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="111.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>70000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>80000</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>90000</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>110000</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>2000</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>90000</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" t="str">
+        <f>_xlfn.CONCAT("('",B26,"',",C26,",",D26,",",E26,",",F26,",'",G26,"'),")</f>
+        <v>('benzyna 1.6',1,1,90000,1,'Skrzynia manuala, napęd FWD, zużycie paliwa średnie: 5.2 l/100 km, średnia emisja CO2: 115.0 g/km.'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>95000</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" ref="H27:H51" si="0">_xlfn.CONCAT("('",B27,"',",C27,",",D27,",",E27,",",F27,",'",G27,"'),")</f>
+        <v>('benzyna 2.0',1,1,95000,1,'Skrzynia manuala, napęd FWD, zużycie paliwa średnie: 4.6 l/100 km, średnia emisja CO2: 119.0 g/km.'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>100000</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>('diesel 1.8',1,1,100000,1,'Skrzynia manuala, napęd FWD, zużycie paliwa średnie: 4.3 l/100 km, średnia emisja CO2: 125.0 g/km.'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>120000</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>('diesel 2.0',1,1,120000,1,'Skrzynia automatyczna, napęd RWD, zużycie paliwa średnie: 4.5 l/100 km, średnia emisja CO2: 127.0 g/km.'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>140000</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>('elektryczny',1,1,140000,1,'Skrzynia automatyczna, napęd AWD, zużycie prądu 15 kWh/100 km'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>10000</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>('awd',1,2,10000,1,'awd'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>12000</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>('fwd',1,2,12000,1,'fwd'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2000</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>('czarny',1,3,2000,1,'Czarny to synonim uniwersalności, a zarazem elegancja'),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>2000</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>('srebrny',1,3,2000,1,'Srebrny to synonim dostatku i prestiżu'),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>2000</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>51</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>('siwy',1,3,2000,1,'Szary to rozwaga i ostrożność'),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>26</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>2000</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>('zielony',1,3,2000,1,'Jeśli przywiązujesz wagę do walorów estetycznych ten kolor jest dla Ciebie!'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>2000</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>53</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>('żółty',1,3,2000,1,'Jesteś łowcą przygód? Żóły to jest to!'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>3000</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>('czerwony',1,3,3000,1,'Lubisz wyróżniać się w tłumie? Ten kolor jest idealny dla Ciebie!'),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>2000</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>('letnie 17'',1,4,2000,1,'Fenomenalna przyczepność, krótka droga hamowania'),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>3500</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>('letnie 18'',1,4,3500,1,'Fenomenalna przyczepność, krótka droga hamowania'),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>1000</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>('przyciemniane szyby',1,5,1000,0,'Przyciemnianie szyb poprawia komfort jazdy, zabezpiecza auto przed nagrzewaniem'),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>3000</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>60</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>('listwy chrom',1,5,3000,0,'Chromowane listwy wykonane z polerowanej stali nierdzewnej dodadzą elegancji oraz podkreślą wyjątkowy charakter Twojego auta'),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>1000</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v>('relingi',1,5,1000,0,'Relingi dachowe to element, który znacząco ułatwia montaż dodatkowego bagażnika na dachu samochodu'),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>500</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>62</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="0"/>
+        <v>('przednia dokładka zewnętrzna',1,5,500,0,'Dokładka wykonana jest z włókna węglowego i jest w błyszczącym wykończeniu'),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>53</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>500</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="0"/>
+        <v>('tylna dokładka zewnętrzna',1,5,500,0,'Dokładka wykonana jest z włókna węglowego i jest w błyszczącym wykończeniu'),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>7000</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="0"/>
+        <v>('skórzana',1,6,7000,1,'skórzana'),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>66</v>
+      </c>
+      <c r="B47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>3000</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>27</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="0"/>
+        <v>('ekoskóra',1,6,3000,1,'ekoskóra'),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>1000</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="0"/>
+        <v>('Materiał',1,6,1000,1,'Materiał'),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>74</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>2000</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="0"/>
+        <v>('Park Assist',1,7,2000,0,'System wspomagający parkowanie samochodów, cały manewr jest wykonywany automatycznie'),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>75</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>3000</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="0"/>
+        <v>('Navigation',1,7,3000,0,'Dożywotnia aktualizacja map, informacja o parkingach '),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>7</v>
+      </c>
+      <c r="E51">
+        <v>1000</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>66</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="0"/>
+        <v>('Power Seats',1,7,1000,0,'Elektryczna regulacja fotela kierowcy, zapamiętuje do trzech ustawień'),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" t="s">
+        <v>40</v>
+      </c>
+      <c r="G57" t="s">
+        <v>41</v>
+      </c>
+      <c r="H57" t="s">
+        <v>36</v>
+      </c>
+      <c r="I57" t="s">
+        <v>39</v>
+      </c>
+      <c r="J57" t="s">
+        <v>42</v>
+      </c>
+      <c r="K57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>90000</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>95000</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>100000</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>4</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>120000</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>5</v>
+      </c>
+      <c r="F62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>140000</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>6</v>
+      </c>
+      <c r="F63" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <v>10000</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <v>7</v>
+      </c>
+      <c r="F64" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>2</v>
+      </c>
+      <c r="I64">
+        <v>12000</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E65">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>3</v>
+      </c>
+      <c r="I65">
+        <v>2000</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E66">
+        <v>9</v>
+      </c>
+      <c r="F66" t="s">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>3</v>
+      </c>
+      <c r="I66">
+        <v>2000</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E67">
+        <v>10</v>
+      </c>
+      <c r="F67" t="s">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>3</v>
+      </c>
+      <c r="I67">
+        <v>2000</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E68">
+        <v>11</v>
+      </c>
+      <c r="F68" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>3</v>
+      </c>
+      <c r="I68">
+        <v>2000</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E69">
+        <v>12</v>
+      </c>
+      <c r="F69" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>3</v>
+      </c>
+      <c r="I69">
+        <v>2000</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E70">
+        <v>13</v>
+      </c>
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>3</v>
+      </c>
+      <c r="I70">
+        <v>3000</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E71">
+        <v>14</v>
+      </c>
+      <c r="F71" t="s">
+        <v>55</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>4</v>
+      </c>
+      <c r="I71">
+        <v>2000</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s">
+        <v>57</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>4</v>
+      </c>
+      <c r="I72">
+        <v>3500</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>16</v>
+      </c>
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>5</v>
+      </c>
+      <c r="I73">
+        <v>1000</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E74">
+        <v>17</v>
+      </c>
+      <c r="F74" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>5</v>
+      </c>
+      <c r="I74">
+        <v>3000</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E75">
+        <v>18</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>5</v>
+      </c>
+      <c r="I75">
+        <v>1000</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E76">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>5</v>
+      </c>
+      <c r="I76">
+        <v>500</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E77">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>5</v>
+      </c>
+      <c r="I77">
+        <v>500</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E78">
+        <v>21</v>
+      </c>
+      <c r="F78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>6</v>
+      </c>
+      <c r="I78">
+        <v>7000</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E79">
+        <v>22</v>
+      </c>
+      <c r="F79" t="s">
+        <v>27</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>6</v>
+      </c>
+      <c r="I79">
+        <v>3000</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E80">
+        <v>23</v>
+      </c>
+      <c r="F80" t="s">
+        <v>28</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>6</v>
+      </c>
+      <c r="I80">
+        <v>1000</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E81">
+        <v>24</v>
+      </c>
+      <c r="F81" t="s">
+        <v>29</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>7</v>
+      </c>
+      <c r="I81">
+        <v>2000</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E82">
+        <v>25</v>
+      </c>
+      <c r="F82" t="s">
+        <v>31</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>7</v>
+      </c>
+      <c r="I82">
+        <v>3000</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E83">
+        <v>26</v>
+      </c>
+      <c r="F83" t="s">
+        <v>32</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>7</v>
+      </c>
+      <c r="I83">
+        <v>1000</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A25:F51" xr:uid="{D05637BF-DA77-47CE-B145-BF447AC71CC8}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>